<commit_message>
Implemented pooling tests for protocols: transfer, sampleQC, libraryPrep and normalization
</commit_message>
<xml_diff>
--- a/backend/fms_core/tests/valid_templates/Library_preparation_v3_10_0.xlsx
+++ b/backend/fms_core/tests/valid_templates/Library_preparation_v3_10_0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sballesteros/Documents/Freezeman/freezeman/backend/fms_core/tests/valid_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37273D9D-4A39-0E42-B49E-4759F7E52C91}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7002E4B-9B6E-534F-81BC-36FA7AB05938}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Library Batch" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2514" uniqueCount="2445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2525" uniqueCount="2450">
   <si>
     <t>Library Preparation Template</t>
   </si>
@@ -7403,6 +7403,21 @@
   </si>
   <si>
     <t>3.10.0</t>
+  </si>
+  <si>
+    <t>PoolContainerSourceLibraryPrep</t>
+  </si>
+  <si>
+    <t>Container4Library4</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Index_4</t>
+  </si>
+  <si>
+    <t>Library 4 Comment</t>
   </si>
 </sst>
 </file>
@@ -7585,7 +7600,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -7645,6 +7660,7 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8046,7 +8062,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMN384"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -10759,12 +10775,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P480"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29.6640625" style="1" customWidth="1"/>
-    <col min="2" max="3" width="24.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29" style="1" customWidth="1"/>
     <col min="4" max="4" width="25.83203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="27.6640625" customWidth="1"/>
     <col min="6" max="7" width="28.5" customWidth="1"/>
@@ -11008,10 +11027,41 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A8" s="21"/>
+      <c r="A8" s="21" t="s">
+        <v>2422</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>2445</v>
+      </c>
       <c r="D8" s="21"/>
-      <c r="H8" s="22"/>
+      <c r="E8" s="41" t="s">
+        <v>2446</v>
+      </c>
+      <c r="G8" s="41" t="s">
+        <v>2446</v>
+      </c>
+      <c r="H8" s="22" t="s">
+        <v>1632</v>
+      </c>
       <c r="J8" s="22"/>
+      <c r="K8" s="1" t="s">
+        <v>2447</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>2447</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="N8" s="39" t="s">
+        <v>2448</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>1248</v>
+      </c>
+      <c r="P8" s="39" t="s">
+        <v>2449</v>
+      </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="21"/>
@@ -13848,8 +13898,8 @@
   </sheetData>
   <dataValidations count="2">
     <dataValidation operator="equal" allowBlank="1" showErrorMessage="1" sqref="D6:D480" xr:uid="{D0E09EEB-28FB-0148-B952-B3C4601A29E5}"/>
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="N8:N384" xr:uid="{BBC63848-808C-3841-A377-DD5DE144DE8B}">
-      <formula1>INDIRECT(SUBSTITUTE(M8," ","_"))</formula1>
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="N9:N384" xr:uid="{BBC63848-808C-3841-A377-DD5DE144DE8B}">
+      <formula1>INDIRECT(SUBSTITUTE(M9," ","_"))</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>